<commit_message>
Fixed error where program tries to open "ATT.xlsx". Changed to "Attendance.xlsx".
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>Number</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>03:52 PM</t>
+  </si>
+  <si>
+    <t>04:22 PM</t>
   </si>
   <si>
     <t>node .js</t>
@@ -556,7 +559,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD12"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
       <selection activeCell="AB10" sqref="AB2:AB10"/>
@@ -915,16 +918,19 @@
       <c r="AB8" t="s">
         <v>61</v>
       </c>
+      <c r="AD8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="9" spans="1:30">
       <c r="A9" t="n">
         <v>321321321</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AA9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AC9" t="s">
         <v>58</v>
@@ -935,86 +941,87 @@
         <v>654654654</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="M10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="P10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Q10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="S10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="U10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="V10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="W10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="X10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Y10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="Z10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AA10" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:30"/>
-    <row r="12" spans="1:30"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Fixed program crashing when excel file is open (permission denied). Added warning for user to understand the issue. Removed "Excel Work.py" and "Plotting Attendance.py".
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
   <si>
     <t>Number</t>
   </si>
@@ -168,6 +168,9 @@
     <t>08:26 PM</t>
   </si>
   <si>
+    <t>04:47 PM</t>
+  </si>
+  <si>
     <t>name nom</t>
   </si>
   <si>
@@ -189,13 +192,13 @@
     <t>03:50 PM</t>
   </si>
   <si>
-    <t>04:47 PM</t>
-  </si>
-  <si>
     <t>06:04 PM</t>
   </si>
   <si>
     <t>turtwig overgrow</t>
+  </si>
+  <si>
+    <t>04:48 PM</t>
   </si>
   <si>
     <t>sql database</t>
@@ -559,7 +562,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD10"/>
+  <dimension ref="A1:AD12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
       <selection activeCell="AB10" sqref="AB2:AB10"/>
@@ -806,13 +809,16 @@
       <c r="AC3" t="s">
         <v>49</v>
       </c>
+      <c r="AD3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:30">
       <c r="A4" s="3" t="n">
         <v>796448521</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
         <v>31</v>
@@ -839,7 +845,7 @@
         <v>0.536805555555556</v>
       </c>
       <c r="S4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AC4" t="s">
         <v>45</v>
@@ -850,7 +856,7 @@
         <v>741852963</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
         <v>31</v>
@@ -862,7 +868,7 @@
         <v>43</v>
       </c>
       <c r="AC5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:30">
@@ -870,7 +876,7 @@
         <v>604604604</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
@@ -879,13 +885,13 @@
         <v>41</v>
       </c>
       <c r="Y6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Z6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AA6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="AB6" t="s">
         <v>44</v>
@@ -904,22 +910,25 @@
       <c r="X7" t="s">
         <v>41</v>
       </c>
+      <c r="AD7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:30">
       <c r="A8" s="3" t="n">
         <v>123123123</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AA8" t="s">
         <v>43</v>
       </c>
       <c r="AB8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AD8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:30">
@@ -927,10 +936,10 @@
         <v>321321321</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AA9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AC9" t="s">
         <v>58</v>
@@ -941,87 +950,89 @@
         <v>654654654</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="N10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="P10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Q10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="R10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="S10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="T10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="U10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="V10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="W10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="X10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Y10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="Z10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AA10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AD10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
+    <row r="11" spans="1:30"/>
+    <row r="12" spans="1:30"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Fixed bugs, improved UI
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:workbookPr codeName="ThisWorkbook"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Attendance" sheetId="1" r:id="rId1"/>
-    <s:sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <s:sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-  </s:sheets>
-  <s:definedNames/>
-  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
-</s:workbook>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr codeName="ThisWorkbook"/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Attendance" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
   <si>
     <t>Number</t>
   </si>
@@ -108,6 +108,18 @@
     <t>August 31 2016</t>
   </si>
   <si>
+    <t>November 04 2016</t>
+  </si>
+  <si>
+    <t>November 05 2016</t>
+  </si>
+  <si>
+    <t>November 12 2016</t>
+  </si>
+  <si>
+    <t>April 22 2017</t>
+  </si>
+  <si>
     <t>monty python</t>
   </si>
   <si>
@@ -159,6 +171,15 @@
     <t>10:49 AM</t>
   </si>
   <si>
+    <t>06:12 PM</t>
+  </si>
+  <si>
+    <t>08:58 AM</t>
+  </si>
+  <si>
+    <t>05:21 PM</t>
+  </si>
+  <si>
     <t>darkest coffee</t>
   </si>
   <si>
@@ -171,18 +192,33 @@
     <t>04:47 PM</t>
   </si>
   <si>
+    <t>06:17 PM</t>
+  </si>
+  <si>
+    <t>08:54 AM</t>
+  </si>
+  <si>
+    <t>09:50 PM</t>
+  </si>
+  <si>
     <t>name nom</t>
   </si>
   <si>
     <t>06:44 PM</t>
   </si>
   <si>
+    <t>09:00 AM</t>
+  </si>
+  <si>
     <t>rubys perls</t>
   </si>
   <si>
     <t>08:25 PM</t>
   </si>
   <si>
+    <t>06:22 PM</t>
+  </si>
+  <si>
     <t>x codes</t>
   </si>
   <si>
@@ -216,10 +252,43 @@
     <t>05:53 PM</t>
   </si>
   <si>
+    <t>08:59 AM</t>
+  </si>
+  <si>
     <t>a d</t>
   </si>
   <si>
     <t>03:05 PM</t>
+  </si>
+  <si>
+    <t>08:56 AM</t>
+  </si>
+  <si>
+    <t>jen sull</t>
+  </si>
+  <si>
+    <t>leon fa</t>
+  </si>
+  <si>
+    <t>aren't you 40</t>
+  </si>
+  <si>
+    <t>leon ar;t 40</t>
+  </si>
+  <si>
+    <t>john set</t>
+  </si>
+  <si>
+    <t>;l kk;</t>
+  </si>
+  <si>
+    <t>04:30 PM</t>
+  </si>
+  <si>
+    <t>as 213</t>
+  </si>
+  <si>
+    <t>04:32 PM</t>
   </si>
 </sst>
 </file>
@@ -259,16 +328,15 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="18" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -562,24 +630,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AD12"/>
+  <dimension ref="A1:AH18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
-      <selection activeCell="AB10" sqref="AB2:AB10"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="AH2" sqref="AH2:AH3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.42578125" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="12"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="1" width="15.7109375"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="1" width="11.28515625"/>
-    <col customWidth="1" max="5" min="5" style="1" width="11.140625"/>
-    <col bestFit="1" customWidth="1" max="10" min="10" style="1" width="14.140625"/>
-    <col bestFit="1" customWidth="1" max="25" min="25" style="1" width="15"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="1" width="12"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="4" width="15.7109375"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="4" width="11.28515625"/>
+    <col customWidth="1" max="5" min="5" style="4" width="11.140625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="4" width="14.140625"/>
+    <col bestFit="1" customWidth="1" max="25" min="25" style="4" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:34">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -588,31 +656,31 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" t="s">
@@ -669,370 +737,510 @@
       <c r="AD1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:30">
-      <c r="A2" s="3" t="n">
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34">
+      <c r="A2" t="n">
         <v>123456789</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>0.411805555555556</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="3" t="n">
         <v>0.453472222222223</v>
       </c>
-      <c r="F2" s="4" t="n">
+      <c r="F2" s="3" t="n">
         <v>0.495138888888889</v>
       </c>
-      <c r="G2" s="4" t="n">
+      <c r="G2" s="3" t="n">
         <v>0.536805555555556</v>
       </c>
-      <c r="H2" s="4" t="n">
+      <c r="H2" s="3" t="n">
         <v>0.5784722222222231</v>
       </c>
-      <c r="I2" s="4" t="n">
+      <c r="I2" s="3" t="n">
         <v>0.620138888888889</v>
       </c>
-      <c r="J2" s="4" t="n">
+      <c r="J2" s="3" t="n">
         <v>0.661805555555556</v>
       </c>
-      <c r="K2" s="4" t="n">
+      <c r="K2" s="3" t="n">
         <v>0.7034722222222231</v>
       </c>
-      <c r="L2" s="4" t="n">
+      <c r="L2" s="3" t="n">
         <v>0.745138888888889</v>
       </c>
-      <c r="M2" s="4" t="n">
+      <c r="M2" s="3" t="n">
         <v>0.786805555555556</v>
       </c>
-      <c r="N2" s="4" t="n">
+      <c r="N2" s="3" t="n">
         <v>0.8284722222222222</v>
       </c>
       <c r="O2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="P2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="Q2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="R2" t="s">
+        <v>39</v>
+      </c>
+      <c r="S2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34">
+      <c r="A3" t="n">
+        <v>543543543</v>
+      </c>
+      <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>0.411805555555556</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>0.453472222222223</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0.495138888888889</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="H3" s="3" t="n">
+        <v>0.5784722222222231</v>
+      </c>
+      <c r="I3" s="3" t="n">
+        <v>0.620138888888889</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>0.661805555555556</v>
+      </c>
+      <c r="K3" s="3" t="n">
+        <v>0.7034722222222231</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>0.745138888888889</v>
+      </c>
+      <c r="M3" s="3" t="n">
+        <v>0.786805555555556</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>55</v>
+      </c>
+      <c r="S3" s="3" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="U3" s="3" t="n"/>
+      <c r="AC3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34">
+      <c r="A4" t="n">
+        <v>796448521</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
         <v>35</v>
       </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>37</v>
-      </c>
-      <c r="U2" t="s">
-        <v>38</v>
-      </c>
-      <c r="V2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" t="s">
-        <v>40</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="D4" s="3" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="J4" s="3" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="O4" s="3" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="Q4" s="3" t="n">
+        <v>0.536805555555556</v>
+      </c>
+      <c r="S4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
+      <c r="A5" t="n">
+        <v>741852963</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W5" t="s">
         <v>41</v>
       </c>
-      <c r="Y2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC2" t="s">
+      <c r="AA5" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34">
+      <c r="A6" t="n">
+        <v>604604604</v>
+      </c>
+      <c r="B6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
+      </c>
+      <c r="X6" t="s">
         <v>45</v>
       </c>
-      <c r="AD2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30">
-      <c r="A3" s="3" t="n">
-        <v>543543543</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="Y6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34">
+      <c r="A7" t="n">
+        <v>789789789</v>
+      </c>
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X7" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34">
+      <c r="A8" t="n">
+        <v>123123123</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA8" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="4" t="n">
-        <v>0.411805555555556</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>0.453472222222223</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>0.495138888888889</v>
-      </c>
-      <c r="G3" s="4" t="n">
-        <v>0.536805555555556</v>
-      </c>
-      <c r="H3" s="4" t="n">
-        <v>0.5784722222222231</v>
-      </c>
-      <c r="I3" s="4" t="n">
-        <v>0.620138888888889</v>
-      </c>
-      <c r="J3" s="4" t="n">
-        <v>0.661805555555556</v>
-      </c>
-      <c r="K3" s="4" t="n">
-        <v>0.7034722222222231</v>
-      </c>
-      <c r="L3" s="4" t="n">
-        <v>0.745138888888889</v>
-      </c>
-      <c r="M3" s="4" t="n">
-        <v>0.786805555555556</v>
-      </c>
-      <c r="O3" s="4" t="n">
-        <v>0.536805555555556</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" s="4" t="n">
-        <v>0.536805555555556</v>
-      </c>
-      <c r="U3" s="4" t="n"/>
-      <c r="AC3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30">
-      <c r="A4" s="3" t="n">
-        <v>796448521</v>
-      </c>
-      <c r="B4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>0.536805555555556</v>
-      </c>
-      <c r="F4" s="4" t="n">
-        <v>0.536805555555556</v>
-      </c>
-      <c r="H4" s="4" t="n">
-        <v>0.536805555555556</v>
-      </c>
-      <c r="J4" s="4" t="n">
-        <v>0.536805555555556</v>
-      </c>
-      <c r="N4" s="4" t="n">
-        <v>0.536805555555556</v>
-      </c>
-      <c r="O4" s="4" t="n">
-        <v>0.536805555555556</v>
-      </c>
-      <c r="Q4" s="4" t="n">
-        <v>0.536805555555556</v>
-      </c>
-      <c r="S4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30">
-      <c r="A5" s="3" t="n">
-        <v>741852963</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="W5" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30">
-      <c r="A6" s="3" t="n">
-        <v>604604604</v>
-      </c>
-      <c r="B6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="X6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>57</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30">
-      <c r="A7" s="3" t="n">
-        <v>789789789</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="X7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30">
-      <c r="A8" s="3" t="n">
-        <v>123123123</v>
-      </c>
-      <c r="B8" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA8" t="s">
-        <v>43</v>
-      </c>
       <c r="AB8" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="AD8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34">
       <c r="A9" t="n">
         <v>321321321</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
       </c>
       <c r="AA9" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="AC9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30">
+        <v>70</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34">
       <c r="A10" t="n">
         <v>654654654</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" t="s">
+        <v>80</v>
+      </c>
+      <c r="M10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N10" t="s">
+        <v>80</v>
+      </c>
+      <c r="O10" t="s">
+        <v>80</v>
+      </c>
+      <c r="P10" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>80</v>
+      </c>
+      <c r="R10" t="s">
+        <v>80</v>
+      </c>
+      <c r="S10" t="s">
+        <v>80</v>
+      </c>
+      <c r="T10" t="s">
+        <v>80</v>
+      </c>
+      <c r="U10" t="s">
+        <v>80</v>
+      </c>
+      <c r="V10" t="s">
+        <v>80</v>
+      </c>
+      <c r="W10" t="s">
+        <v>80</v>
+      </c>
+      <c r="X10" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34">
+      <c r="A11" t="n">
+        <v>654654654</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34">
+      <c r="A12" t="n">
+        <v>982313456</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34">
+      <c r="A13" t="n">
+        <v>789654332</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34">
+      <c r="A14" t="n">
+        <v>763194463</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34">
+      <c r="A15" t="n">
+        <v>789465421</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34">
+      <c r="A16" t="n">
+        <v>123000000</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:34">
+      <c r="A17" t="n">
+        <v>741000144</v>
+      </c>
+      <c r="B17" t="s">
         <v>67</v>
       </c>
-      <c r="E10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I10" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" t="s">
-        <v>67</v>
-      </c>
-      <c r="K10" t="s">
-        <v>67</v>
-      </c>
-      <c r="L10" t="s">
-        <v>67</v>
-      </c>
-      <c r="M10" t="s">
-        <v>67</v>
-      </c>
-      <c r="N10" t="s">
-        <v>67</v>
-      </c>
-      <c r="O10" t="s">
-        <v>67</v>
-      </c>
-      <c r="P10" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>67</v>
-      </c>
-      <c r="R10" t="s">
-        <v>67</v>
-      </c>
-      <c r="S10" t="s">
-        <v>67</v>
-      </c>
-      <c r="T10" t="s">
-        <v>67</v>
-      </c>
-      <c r="U10" t="s">
-        <v>67</v>
-      </c>
-      <c r="V10" t="s">
-        <v>67</v>
-      </c>
-      <c r="W10" t="s">
-        <v>67</v>
-      </c>
-      <c r="X10" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30"/>
-    <row r="12" spans="1:30"/>
+      <c r="AH17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:34">
+      <c r="A18" t="n">
+        <v>100300400</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
@@ -1051,7 +1259,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1069,7 +1277,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>